<commit_message>
The leave request template has a code column added, while the permission request template has a dropdown added for absences (alpha).
</commit_message>
<xml_diff>
--- a/wwwroot/uploads/TemplateForm/TemplateLeaveRequest.xlsx
+++ b/wwwroot/uploads/TemplateForm/TemplateLeaveRequest.xlsx
@@ -20,7 +20,7 @@
     <author>ismail - [2010]</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
     <author>ismail - [2010]</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>No</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>Rencana Melahirkan Pada 30 Januari</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>0774/SS/PERS-JKT/I/2025</t>
+  </si>
+  <si>
+    <t>0774/SI/PERS-JKT/I/2025</t>
+  </si>
+  <si>
+    <t>0774/SC/PERS-JKT/I/2025</t>
   </si>
 </sst>
 </file>
@@ -154,9 +166,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-13809]dd/mm/yyyy;@"/>
-    <numFmt numFmtId="168" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +188,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -198,10 +216,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,24 +522,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="2" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,21 +550,24 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F69">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G69">
       <formula1>"Cuti, Cuti Bersama, Cuti Melahirkan, Cuti Menikah"</formula1>
     </dataValidation>
   </dataValidations>
@@ -557,10 +579,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="A1:G5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,13 +590,14 @@
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -585,19 +608,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -607,20 +633,23 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
-        <v>45636</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45667</v>
+      </c>
+      <c r="F2">
         <v>0.5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -630,20 +659,23 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
-        <v>45652</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45683</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -653,20 +685,23 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2">
-        <v>45604</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45299</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -676,22 +711,25 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2">
-        <v>45324</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2">
+        <v>45292</v>
+      </c>
+      <c r="F5">
         <v>90</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5">
       <formula1>"Cuti, Cuti Bersama, Cuti Melahirkan, Cuti Menikah"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update template leave request
</commit_message>
<xml_diff>
--- a/wwwroot/uploads/TemplateForm/TemplateLeaveRequest.xlsx
+++ b/wwwroot/uploads/TemplateForm/TemplateLeaveRequest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,9 @@
 - Cuti
 - Cuti Bersama
 - Cuti Melahirkan
-- Cuti Menikah</t>
+- Cuti Menikah
+- Alpha (Potong Gaji)
+- Alpha (Potong Cuti)</t>
         </r>
       </text>
     </comment>
@@ -524,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,8 +569,8 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G69">
-      <formula1>"Cuti, Cuti Bersama, Cuti Melahirkan, Cuti Menikah"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576">
+      <formula1>"Cuti, Cuti Bersama, Cuti Melahirkan, Cuti Menikah, Alpha (Potong Gaji), Alpha (Potong Cuti)"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -581,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,8 +731,8 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5">
-      <formula1>"Cuti, Cuti Bersama, Cuti Melahirkan, Cuti Menikah"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576">
+      <formula1>"Cuti, Cuti Bersama, Cuti Melahirkan, Cuti Menikah, Alpha (Potong Gaji), Alpha (Potong Cuti)"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>